<commit_message>
test new version 2.4.0
</commit_message>
<xml_diff>
--- a/Examples/Dictionary/Input/Exp61_RatingsTable.xlsx
+++ b/Examples/Dictionary/Input/Exp61_RatingsTable.xlsx
@@ -951,7 +951,7 @@
     <row r="7">
       <c r="A7" s="17" t="inlineStr">
         <is>
-          <t>ESTIMATED RESULTS</t>
+          <t>ESTIMATED TOTALS AND PRIORITIES</t>
         </is>
       </c>
       <c r="B7" s="17" t="inlineStr"/>
@@ -1060,7 +1060,25 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="18">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A5</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A11:A13</formula1>
+    </dataValidation>
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=rating_scales!A3:A5</formula1>
     </dataValidation>

</xml_diff>